<commit_message>
Commit before configuring .env
Search and cart is incomplete till now.
</commit_message>
<xml_diff>
--- a/testData/testData_user.xlsx
+++ b/testData/testData_user.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="8692" activeTab="3"/>
+    <workbookView windowWidth="19200" windowHeight="7972" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
   <si>
     <t>Email</t>
   </si>
@@ -128,7 +128,7 @@
     <t>COMP-45</t>
   </si>
   <si>
-    <t>8 GB</t>
+    <t>4GB [+$20.00]</t>
   </si>
   <si>
     <t>400 GB</t>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>2.5 GHz Intel Pentium Dual-Core E2200</t>
+  </si>
+  <si>
+    <t>8GB [+$60.00]</t>
   </si>
   <si>
     <t>Vista Premium</t>
@@ -1390,8 +1393,8 @@
   <sheetPr/>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="6"/>
@@ -1512,16 +1515,16 @@
         <v>40</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K4" s="5">
         <v>1315</v>
@@ -1536,10 +1539,10 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K5" s="5">
         <v>1249</v>
@@ -1554,10 +1557,10 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K6" s="5">
         <v>1340</v>
@@ -1572,22 +1575,22 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K7" s="5">
         <v>850</v>
@@ -1611,7 +1614,7 @@
   <sheetPr/>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1645,28 +1648,28 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1674,75 +1677,75 @@
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J2" s="1">
         <v>10001</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J3" s="1">
         <v>3496</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
.env configured in early stage. search and cart is not finished yet
</commit_message>
<xml_diff>
--- a/testData/testData_user.xlsx
+++ b/testData/testData_user.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7972" activeTab="2"/>
+    <workbookView windowWidth="19200" windowHeight="8692" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="79">
   <si>
     <t>Email</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Signature</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>sakib75@gmail.com</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
   </si>
   <si>
     <t>Brain station 23</t>
-  </si>
-  <si>
-    <t>admin</t>
   </si>
   <si>
     <t>steve_gates@nopCommerce.com</t>
@@ -1251,24 +1245,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F1"/>
+      <selection activeCell="F1" sqref="F$1:F$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="18.2389380530973" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.1238938053097" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.716814159292" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.6991150442478" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.79646017699115" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.92920353982301" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="1" ht="15.75" spans="1:6">
+    <row r="1" s="8" customFormat="1" ht="15.75" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1284,28 +1277,22 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1">
-        <v>123456</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1317,24 +1304,23 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="29.7256637168142" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.1238938053097" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.716814159292" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.6991150442478" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.79646017699115" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.92920353982301" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="1" ht="15.75" spans="1:6">
+    <row r="1" s="8" customFormat="1" ht="15.75" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1350,36 +1336,27 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1">
-        <v>123456</v>
       </c>
     </row>
   </sheetData>
@@ -1393,7 +1370,7 @@
   <sheetPr/>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1411,63 +1388,63 @@
   <sheetData>
     <row r="1" s="4" customFormat="1" ht="15.75" spans="1:13">
       <c r="A1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="K2" s="5">
         <v>1110</v>
@@ -1482,16 +1459,16 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="K3" s="5">
         <v>55</v>
@@ -1506,25 +1483,25 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="F4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="K4" s="5">
         <v>1315</v>
@@ -1539,10 +1516,10 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K5" s="5">
         <v>1249</v>
@@ -1557,10 +1534,10 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K6" s="5">
         <v>1340</v>
@@ -1575,22 +1552,22 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="K7" s="5">
         <v>850</v>
@@ -1648,104 +1625,104 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="J2" s="1">
         <v>10001</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="J3" s="1">
         <v>3496</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cart page product verification
</commit_message>
<xml_diff>
--- a/testData/testData_user.xlsx
+++ b/testData/testData_user.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="8692" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="7972" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t>Email</t>
   </si>
@@ -164,10 +164,19 @@
     <t>DS_VA3_PC</t>
   </si>
   <si>
+    <t>1249</t>
+  </si>
+  <si>
+    <t>3240</t>
+  </si>
+  <si>
     <t>HP Spectre XT Pro UltraBook</t>
   </si>
   <si>
     <t>HP_SPX_UB</t>
+  </si>
+  <si>
+    <t>1340</t>
   </si>
   <si>
     <t>Bose Home Speaker 500</t>
@@ -911,16 +920,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1306,7 +1315,7 @@
   <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -1370,8 +1379,8 @@
   <sheetPr/>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="6"/>
@@ -1521,53 +1530,51 @@
       <c r="C5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="5">
-        <v>1249</v>
+      <c r="K5" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="L5" s="5">
         <v>6</v>
       </c>
-      <c r="M5" s="5">
-        <f>540*L5</f>
-        <v>3240</v>
+      <c r="M5" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="5">
-        <v>1340</v>
+        <v>47</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="L6" s="5">
         <v>1</v>
       </c>
       <c r="M6" s="5">
-        <f>K6*L6</f>
         <v>1340</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="K7" s="5">
         <v>850</v>
@@ -1625,28 +1632,28 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1654,75 +1661,75 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J2" s="1">
         <v>10001</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J3" s="1">
         <v>3496</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Push before major changes
</commit_message>
<xml_diff>
--- a/testData/testData_user.xlsx
+++ b/testData/testData_user.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="80">
   <si>
     <t>Email</t>
   </si>
@@ -98,10 +98,10 @@
     <t>Software</t>
   </si>
   <si>
-    <t>Serial No File Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Color </t>
+    <t>Serial File Path</t>
+  </si>
+  <si>
+    <t>Color</t>
   </si>
   <si>
     <t>Price</t>
@@ -113,6 +113,30 @@
     <t>Total Price</t>
   </si>
   <si>
+    <t>Microsoft Surface Pro 9</t>
+  </si>
+  <si>
+    <t>COMP_CUST</t>
+  </si>
+  <si>
+    <t>2.5 GHz Intel Pentium Dual-Core E2200</t>
+  </si>
+  <si>
+    <t>8GB [+$60.00]</t>
+  </si>
+  <si>
+    <t>400 GB</t>
+  </si>
+  <si>
+    <t>Vista Premium</t>
+  </si>
+  <si>
+    <t>Microsoft Office</t>
+  </si>
+  <si>
+    <t>Serial No.txt</t>
+  </si>
+  <si>
     <t>Bose QuietComfort 45</t>
   </si>
   <si>
@@ -125,9 +149,6 @@
     <t>4GB [+$20.00]</t>
   </si>
   <si>
-    <t>400 GB</t>
-  </si>
-  <si>
     <t>Silver</t>
   </si>
   <si>
@@ -140,43 +161,16 @@
     <t>Pink</t>
   </si>
   <si>
-    <t>Microsoft Surface Pro 9</t>
-  </si>
-  <si>
-    <t>COMP_CUST</t>
-  </si>
-  <si>
-    <t>2.5 GHz Intel Pentium Dual-Core E2200</t>
-  </si>
-  <si>
-    <t>8GB [+$60.00]</t>
-  </si>
-  <si>
-    <t>Vista Premium</t>
-  </si>
-  <si>
-    <t>Microsoft Office</t>
-  </si>
-  <si>
     <t>Digital Storm VANQUISH Custom Performance PC</t>
   </si>
   <si>
     <t>DS_VA3_PC</t>
   </si>
   <si>
-    <t>1249</t>
-  </si>
-  <si>
-    <t>3240</t>
-  </si>
-  <si>
     <t>HP Spectre XT Pro UltraBook</t>
   </si>
   <si>
     <t>HP_SPX_UB</t>
-  </si>
-  <si>
-    <t>1340</t>
   </si>
   <si>
     <t>Bose Home Speaker 500</t>
@@ -909,7 +903,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -931,6 +925,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1270,7 +1267,7 @@
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="1" ht="15.75" spans="1:5">
+    <row r="1" s="9" customFormat="1" ht="15.75" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1329,7 +1326,7 @@
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="1" ht="15.75" spans="1:5">
+    <row r="1" s="9" customFormat="1" ht="15.75" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1379,8 +1376,8 @@
   <sheetPr/>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="$A2:$XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="6"/>
@@ -1440,10 +1437,10 @@
       <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -1452,103 +1449,106 @@
       <c r="F2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="H2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="K2" s="5">
-        <v>1110</v>
+        <v>1315</v>
       </c>
       <c r="L2" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M2" s="5">
         <f>K2*L2</f>
-        <v>2220</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="K3" s="5">
-        <v>55</v>
+        <v>1110</v>
       </c>
       <c r="L3" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M3" s="5">
         <f>K3*L3</f>
-        <v>165</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="J4" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="K4" s="5">
-        <v>1315</v>
+        <v>55</v>
       </c>
       <c r="L4" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M4" s="5">
         <f>K4*L4</f>
-        <v>1315</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="K5" s="8">
+        <v>1249</v>
       </c>
       <c r="L5" s="5">
         <v>6</v>
       </c>
-      <c r="M5" s="5" t="s">
-        <v>45</v>
+      <c r="M5" s="8">
+        <v>3240</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>48</v>
+      <c r="K6" s="8">
+        <v>1340</v>
       </c>
       <c r="L6" s="5">
         <v>1</v>
@@ -1559,22 +1559,22 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="K7" s="5">
         <v>850</v>
@@ -1632,28 +1632,28 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1661,75 +1661,75 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="J2" s="1">
         <v>10001</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="J3" s="1">
         <v>3496</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed major bugs on serarch and cart page
</commit_message>
<xml_diff>
--- a/testData/testData_user.xlsx
+++ b/testData/testData_user.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7972" activeTab="2"/>
+    <workbookView windowWidth="19200" windowHeight="8692" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -1376,8 +1376,8 @@
   <sheetPr/>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="6"/>

</xml_diff>

<commit_message>
Previous order details check added. but not used data driven test. Hardcoded data. will be finished later.
</commit_message>
<xml_diff>
--- a/testData/testData_user.xlsx
+++ b/testData/testData_user.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="8692" activeTab="2"/>
+    <workbookView windowWidth="19200" windowHeight="8692" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
     <sheet name="Admins" sheetId="2" r:id="rId2"/>
     <sheet name="Products" sheetId="3" r:id="rId3"/>
     <sheet name="Addresses" sheetId="4" r:id="rId4"/>
+    <sheet name="Orders" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="93">
   <si>
     <t>Email</t>
   </si>
@@ -270,6 +271,45 @@
   </si>
   <si>
     <t>265-7854</t>
+  </si>
+  <si>
+    <t>Order ID</t>
+  </si>
+  <si>
+    <t>Order Date</t>
+  </si>
+  <si>
+    <t>Order Status</t>
+  </si>
+  <si>
+    <t>Product SKU</t>
+  </si>
+  <si>
+    <t>Product Price</t>
+  </si>
+  <si>
+    <t>Product Qty</t>
+  </si>
+  <si>
+    <t>Product Total Price</t>
+  </si>
+  <si>
+    <t>Order Total Price</t>
+  </si>
+  <si>
+    <t>Thursday, September 25, 2025</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>1,249.00</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
 </sst>
 </file>
@@ -282,7 +322,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +336,12 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -773,154 +819,155 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -929,7 +976,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1259,45 +1306,45 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="18.2389380530973" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1238938053097" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.716814159292" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6991150442478" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.79646017699115" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="18.2389380530973" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.1238938053097" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.716814159292" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.6991150442478" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.79646017699115" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="1" ht="15.75" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="10" customFormat="1" ht="15.75" spans="1:5">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1318,50 +1365,50 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="29.7256637168142" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1238938053097" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.716814159292" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6991150442478" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.79646017699115" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="29.7256637168142" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.1238938053097" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.716814159292" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.6991150442478" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.79646017699115" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="1" ht="15.75" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="10" customFormat="1" ht="15.75" spans="1:5">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1376,213 +1423,213 @@
   <sheetPr/>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" width="43.8672566371681" style="5" customWidth="1"/>
-    <col min="2" max="3" width="20.1061946902655" style="5" customWidth="1"/>
-    <col min="4" max="4" width="31.3982300884956" style="5" customWidth="1"/>
-    <col min="5" max="10" width="20.1061946902655" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8.46902654867257" style="5" customWidth="1"/>
-    <col min="12" max="12" width="4.65486725663717" style="5" customWidth="1"/>
-    <col min="13" max="13" width="10.787610619469" style="5" customWidth="1"/>
-    <col min="14" max="16384" width="9.02654867256637" style="5"/>
+    <col min="1" max="1" width="43.8672566371681" style="1" customWidth="1"/>
+    <col min="2" max="3" width="20.1061946902655" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.3982300884956" style="1" customWidth="1"/>
+    <col min="5" max="10" width="20.1061946902655" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.46902654867257" style="1" customWidth="1"/>
+    <col min="12" max="12" width="4.65486725663717" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.787610619469" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.02654867256637" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" ht="15.75" spans="1:13">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="7" customFormat="1" ht="15.75" spans="1:13">
+      <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="1">
         <v>1315</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="1">
         <v>1</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="1">
         <f>K2*L2</f>
         <v>1315</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="1">
         <v>1110</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="1">
         <v>2</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="1">
         <f>K3*L3</f>
         <v>2220</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="1">
         <v>55</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="1">
         <v>3</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="1">
         <f>K4*L4</f>
         <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="9">
         <v>1249</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="1">
         <v>6</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="9">
         <v>3240</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="9">
         <v>1340</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="1">
         <v>1</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="1">
         <v>1340</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="1">
         <v>850</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="1">
         <v>2</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="1">
         <f>K7*L7</f>
         <v>1700</v>
       </c>
@@ -1604,131 +1651,131 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="11.1238938053097" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.716814159292" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.9203539823009" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.0353982300885" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.4336283185841" style="1" customWidth="1"/>
-    <col min="6" max="7" width="9.05309734513274" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1946902654867" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1238938053097" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.06194690265487" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.3097345132743" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.3805309734513" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.02654867256637" style="1"/>
+    <col min="1" max="1" width="11.1238938053097" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.716814159292" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.9203539823009" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.0353982300885" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.4336283185841" style="4" customWidth="1"/>
+    <col min="6" max="7" width="9.05309734513274" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.1946902654867" style="4" customWidth="1"/>
+    <col min="9" max="9" width="10.1238938053097" style="4" customWidth="1"/>
+    <col min="10" max="10" width="9.06194690265487" style="4" customWidth="1"/>
+    <col min="11" max="11" width="15.3097345132743" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12.3805309734513" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="9.02654867256637" style="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:12">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="4">
         <v>10001</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="4">
         <v>3496</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="4" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1740,4 +1787,97 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="8.92035398230088" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.3008849557522" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7964601769912" style="1" customWidth="1"/>
+    <col min="4" max="4" width="43.8672566371681" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7256637168142" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6548672566372" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.3185840707965" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.0530973451327" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.9823008849558" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.02654867256637" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="Digital Storm VANQUISH Custom Performance PC" tooltip="http://localhost:88/digital-storm-vanquish-custom-performance-pc"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <ignoredErrors>
+    <ignoredError sqref="G2:I2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>